<commit_message>
Revised the MIDI mappings and documentation for the stand-alone effects.   The goal with the stand-alone effects is that each effect running on the SAM would map common controls to HADC-0,1,2 as well as SW-4 (enable)
</commit_message>
<xml_diff>
--- a/examples/SAM/chorus/MIDI Mappings Chorus.xlsx
+++ b/examples/SAM/chorus/MIDI Mappings Chorus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10060" yWindow="2880" windowWidth="25600" windowHeight="18700" tabRatio="500"/>
+    <workbookView xWindow="19400" yWindow="9700" windowWidth="11740" windowHeight="9300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="By Module" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Function</t>
   </si>
@@ -77,10 +77,19 @@
     <t>knob</t>
   </si>
   <si>
-    <t>switch</t>
-  </si>
-  <si>
     <t>Enable</t>
+  </si>
+  <si>
+    <t>knob (HADC-0)</t>
+  </si>
+  <si>
+    <t>switch (SW-4)</t>
+  </si>
+  <si>
+    <t>knob (HADC-1)</t>
+  </si>
+  <si>
+    <t>knob (HADC-2)</t>
   </si>
 </sst>
 </file>
@@ -134,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -167,6 +176,51 @@
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
@@ -179,128 +233,100 @@
       <right style="thin">
         <color auto="1"/>
       </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top style="medium">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
         <color auto="1"/>
       </right>
       <top style="medium">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="135">
+  <cellStyleXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -436,24 +462,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="135">
+  <cellStyles count="151">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -521,6 +564,14 @@
     <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -588,6 +639,14 @@
     <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -917,10 +976,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D2" sqref="D2:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -928,104 +987,93 @@
     <col min="1" max="1" width="29.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
     <col min="3" max="3" width="23.5" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="16.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" ht="16" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16" thickBot="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+    <row r="2" spans="1:4">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>105</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="B3" s="7">
-        <v>55</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>9</v>
+      <c r="D3" s="12" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="13">
-        <v>103</v>
-      </c>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="6">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>10</v>
+      <c r="D4" s="12" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="9">
-        <v>56</v>
-      </c>
-      <c r="C5" s="9" t="s">
+      <c r="A5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="16" thickBot="1">
+      <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <v>58</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="9">
-        <v>57</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1">
-      <c r="A7" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="11">
-        <v>58</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A6:C46">

</xml_diff>